<commit_message>
Attempting to remove makefile changes from pull request
</commit_message>
<xml_diff>
--- a/input/activity/metals/Blast_furnace_iron_production_1850-2014.xlsx
+++ b/input/activity/metals/Blast_furnace_iron_production_1850-2014.xlsx
@@ -1,16 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26709"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ben/mystuff/CEDS/input/activity/metals/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3760" yWindow="460" windowWidth="25040" windowHeight="14320" tabRatio="624"/>
-    <workbookView xWindow="1700" yWindow="1260" windowWidth="24480" windowHeight="13760" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="14320" tabRatio="624"/>
+    <workbookView xWindow="1120" yWindow="1120" windowWidth="24480" windowHeight="13760" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -23,7 +18,7 @@
     <externalReference r:id="rId6"/>
     <externalReference r:id="rId7"/>
   </externalReferences>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1882,11 +1877,6 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -2544,11 +2534,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2132149792"/>
-        <c:axId val="-2132146736"/>
+        <c:axId val="-2037795800"/>
+        <c:axId val="-2037790088"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2132149792"/>
+        <c:axId val="-2037795800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2583,12 +2573,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2132146736"/>
+        <c:crossAx val="-2037790088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2132146736"/>
+        <c:axId val="-2037790088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2633,7 +2623,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2132149792"/>
+        <c:crossAx val="-2037795800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2769,7 +2759,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Notes"/>
@@ -7987,7 +7977,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Pig Iron"/>
@@ -10271,16 +10261,16 @@
   <dimension ref="A1:DZ84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="CE58" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomRight" activeCell="CP82" sqref="CP82"/>
     </sheetView>
     <sheetView topLeftCell="T28" workbookViewId="1">
       <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="19.83203125" customWidth="1"/>
     <col min="2" max="2" width="7.33203125" style="43" customWidth="1"/>
@@ -10294,12 +10284,12 @@
     <col min="124" max="128" width="9.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:130" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:130" s="32" customFormat="1">
       <c r="A1" s="32" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:130" s="32" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:130" s="32" customFormat="1">
       <c r="A2" s="32" t="s">
         <v>0</v>
       </c>
@@ -10308,7 +10298,7 @@
         <v>31914</v>
       </c>
     </row>
-    <row r="3" spans="1:130" s="33" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:130" s="33" customFormat="1">
       <c r="A3" s="33" t="s">
         <v>1</v>
       </c>
@@ -10694,7 +10684,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="4" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:130" ht="15">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -11181,7 +11171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:130" ht="15">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -11669,7 +11659,7 @@
       </c>
       <c r="DZ5" s="9"/>
     </row>
-    <row r="6" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:130" ht="15">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -12157,7 +12147,7 @@
       </c>
       <c r="DZ6" s="9"/>
     </row>
-    <row r="7" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:130" ht="15">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -12666,7 +12656,7 @@
       </c>
       <c r="DZ7" s="9"/>
     </row>
-    <row r="8" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:130" ht="15">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -13178,7 +13168,7 @@
       </c>
       <c r="DZ8" s="9"/>
     </row>
-    <row r="9" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:130" ht="15">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -13690,7 +13680,7 @@
       </c>
       <c r="DZ9" s="9"/>
     </row>
-    <row r="10" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:130" ht="15">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -14202,7 +14192,7 @@
       </c>
       <c r="DZ10" s="9"/>
     </row>
-    <row r="11" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:130" ht="15">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -14706,7 +14696,7 @@
       </c>
       <c r="DZ11" s="9"/>
     </row>
-    <row r="12" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:130" ht="15">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -15218,7 +15208,7 @@
       </c>
       <c r="DZ12" s="9"/>
     </row>
-    <row r="13" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:130" ht="15">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -15727,7 +15717,7 @@
       </c>
       <c r="DZ13" s="9"/>
     </row>
-    <row r="14" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:130" ht="15">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -16215,7 +16205,7 @@
       </c>
       <c r="DZ14" s="9"/>
     </row>
-    <row r="15" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:130" ht="15">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -16724,7 +16714,7 @@
       </c>
       <c r="DZ15" s="9"/>
     </row>
-    <row r="16" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:130" ht="15">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -17212,7 +17202,7 @@
       </c>
       <c r="DZ16" s="9"/>
     </row>
-    <row r="17" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:130" ht="15">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -17724,7 +17714,7 @@
       </c>
       <c r="DZ17" s="9"/>
     </row>
-    <row r="18" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:130" ht="15">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -18236,7 +18226,7 @@
       </c>
       <c r="DZ18" s="9"/>
     </row>
-    <row r="19" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:130" ht="15">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -18724,7 +18714,7 @@
       </c>
       <c r="DZ19" s="9"/>
     </row>
-    <row r="20" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:130" ht="15">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -19236,7 +19226,7 @@
       </c>
       <c r="DZ20" s="9"/>
     </row>
-    <row r="21" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:130" ht="15">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -19748,7 +19738,7 @@
       </c>
       <c r="DZ21" s="9"/>
     </row>
-    <row r="22" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:130" ht="15">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -20260,7 +20250,7 @@
       </c>
       <c r="DZ22" s="9"/>
     </row>
-    <row r="23" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:130" ht="15">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -20772,7 +20762,7 @@
       </c>
       <c r="DZ23" s="9"/>
     </row>
-    <row r="24" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:130" ht="15">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -21260,7 +21250,7 @@
       </c>
       <c r="DZ24" s="9"/>
     </row>
-    <row r="25" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:130" ht="15">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -21772,7 +21762,7 @@
       </c>
       <c r="DZ25" s="9"/>
     </row>
-    <row r="26" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:130" ht="15">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -22279,7 +22269,7 @@
       </c>
       <c r="DZ26" s="9"/>
     </row>
-    <row r="27" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:130" ht="15">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -22767,7 +22757,7 @@
       </c>
       <c r="DZ27" s="9"/>
     </row>
-    <row r="28" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:130" ht="15">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -23279,7 +23269,7 @@
       </c>
       <c r="DZ28" s="9"/>
     </row>
-    <row r="29" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:130" ht="15">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -23788,7 +23778,7 @@
       </c>
       <c r="DZ29" s="9"/>
     </row>
-    <row r="30" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:130" ht="15">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -24276,7 +24266,7 @@
       </c>
       <c r="DZ30" s="9"/>
     </row>
-    <row r="31" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:130" ht="15">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -24788,7 +24778,7 @@
       </c>
       <c r="DZ31" s="9"/>
     </row>
-    <row r="32" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:130" ht="15">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -25276,7 +25266,7 @@
       </c>
       <c r="DZ32" s="9"/>
     </row>
-    <row r="33" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:130" ht="15">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -25780,7 +25770,7 @@
       </c>
       <c r="DZ33" s="9"/>
     </row>
-    <row r="34" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:130" ht="15">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -26268,7 +26258,7 @@
       </c>
       <c r="DZ34" s="9"/>
     </row>
-    <row r="35" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:130" ht="15">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -26780,7 +26770,7 @@
       </c>
       <c r="DZ35" s="9"/>
     </row>
-    <row r="36" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:130" ht="15">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -27268,7 +27258,7 @@
       </c>
       <c r="DZ36" s="9"/>
     </row>
-    <row r="37" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:130" ht="15">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -27756,7 +27746,7 @@
       </c>
       <c r="DZ37" s="9"/>
     </row>
-    <row r="38" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:130" ht="15">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -28244,7 +28234,7 @@
       </c>
       <c r="DZ38" s="9"/>
     </row>
-    <row r="39" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:130" ht="15">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -28732,7 +28722,7 @@
       </c>
       <c r="DZ39" s="9"/>
     </row>
-    <row r="40" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:130" ht="15">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -29220,7 +29210,7 @@
       </c>
       <c r="DZ40" s="9"/>
     </row>
-    <row r="41" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:130" ht="15">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -29708,7 +29698,7 @@
       </c>
       <c r="DZ41" s="9"/>
     </row>
-    <row r="42" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:130" ht="15">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -30220,7 +30210,7 @@
       </c>
       <c r="DZ42" s="9"/>
     </row>
-    <row r="43" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:130" ht="15">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -30708,7 +30698,7 @@
       </c>
       <c r="DZ43" s="9"/>
     </row>
-    <row r="44" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:130" ht="15">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -31220,7 +31210,7 @@
       </c>
       <c r="DZ44" s="9"/>
     </row>
-    <row r="45" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:130" ht="15">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -31708,7 +31698,7 @@
       </c>
       <c r="DZ45" s="9"/>
     </row>
-    <row r="46" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:130" ht="15">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -32217,7 +32207,7 @@
       </c>
       <c r="DZ46" s="9"/>
     </row>
-    <row r="47" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:130" ht="15">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -32705,7 +32695,7 @@
       </c>
       <c r="DZ47" s="9"/>
     </row>
-    <row r="48" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:130" ht="15">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -33193,7 +33183,7 @@
       </c>
       <c r="DZ48" s="9"/>
     </row>
-    <row r="49" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:130" ht="15">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -33681,7 +33671,7 @@
       </c>
       <c r="DZ49" s="9"/>
     </row>
-    <row r="50" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:130" ht="15">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -34169,7 +34159,7 @@
       </c>
       <c r="DZ50" s="9"/>
     </row>
-    <row r="51" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:130" ht="15">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -34681,7 +34671,7 @@
       </c>
       <c r="DZ51" s="9"/>
     </row>
-    <row r="52" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:130" ht="15">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -35193,7 +35183,7 @@
       </c>
       <c r="DZ52" s="9"/>
     </row>
-    <row r="53" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:130" ht="15">
       <c r="A53" t="s">
         <v>51</v>
       </c>
@@ -35681,7 +35671,7 @@
       </c>
       <c r="DZ53" s="9"/>
     </row>
-    <row r="54" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:130" ht="15">
       <c r="A54" t="s">
         <v>52</v>
       </c>
@@ -36169,7 +36159,7 @@
       </c>
       <c r="DZ54" s="9"/>
     </row>
-    <row r="55" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:130" ht="15">
       <c r="A55" t="s">
         <v>53</v>
       </c>
@@ -36657,7 +36647,7 @@
       </c>
       <c r="DZ55" s="9"/>
     </row>
-    <row r="56" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:130" ht="15">
       <c r="A56" t="s">
         <v>54</v>
       </c>
@@ -37145,7 +37135,7 @@
       </c>
       <c r="DZ56" s="9"/>
     </row>
-    <row r="57" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:130" ht="15">
       <c r="A57" t="s">
         <v>55</v>
       </c>
@@ -37633,7 +37623,7 @@
       </c>
       <c r="DZ57" s="9"/>
     </row>
-    <row r="58" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:130" ht="15">
       <c r="A58" t="s">
         <v>56</v>
       </c>
@@ -38145,7 +38135,7 @@
       </c>
       <c r="DZ58" s="9"/>
     </row>
-    <row r="59" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:130" ht="15">
       <c r="A59" t="s">
         <v>57</v>
       </c>
@@ -38654,7 +38644,7 @@
       </c>
       <c r="DZ59" s="9"/>
     </row>
-    <row r="60" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:130" ht="15">
       <c r="A60" t="s">
         <v>58</v>
       </c>
@@ -39142,7 +39132,7 @@
       </c>
       <c r="DZ60" s="9"/>
     </row>
-    <row r="61" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:130" ht="15">
       <c r="A61" t="s">
         <v>59</v>
       </c>
@@ -39630,7 +39620,7 @@
       </c>
       <c r="DZ61" s="9"/>
     </row>
-    <row r="62" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:130" ht="15">
       <c r="A62" t="s">
         <v>60</v>
       </c>
@@ -40142,7 +40132,7 @@
       </c>
       <c r="DZ62" s="9"/>
     </row>
-    <row r="63" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:130" ht="15">
       <c r="A63" s="3" t="s">
         <v>61</v>
       </c>
@@ -40631,7 +40621,7 @@
       </c>
       <c r="DZ63" s="9"/>
     </row>
-    <row r="64" spans="1:130" ht="16" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:130" ht="15">
       <c r="A64" t="s">
         <v>62</v>
       </c>
@@ -41057,7 +41047,7 @@
       </c>
       <c r="DZ64" s="9"/>
     </row>
-    <row r="65" spans="1:130" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:130">
       <c r="A65" s="1" t="s">
         <v>71</v>
       </c>
@@ -41483,7 +41473,7 @@
       </c>
       <c r="DZ65" s="9"/>
     </row>
-    <row r="66" spans="1:130" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:130">
       <c r="CP66" s="2"/>
       <c r="CQ66" s="2"/>
       <c r="CR66" s="2"/>
@@ -41521,7 +41511,7 @@
       <c r="DX66" s="2"/>
       <c r="DZ66" s="9"/>
     </row>
-    <row r="67" spans="1:130" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:130">
       <c r="A67" s="1" t="s">
         <v>66</v>
       </c>
@@ -41944,7 +41934,7 @@
       <c r="DX67" s="2"/>
       <c r="DZ67" s="9"/>
     </row>
-    <row r="68" spans="1:130" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:130" s="1" customFormat="1">
       <c r="A68" s="1" t="s">
         <v>70</v>
       </c>
@@ -42256,7 +42246,7 @@
       </c>
       <c r="DZ68" s="9"/>
     </row>
-    <row r="69" spans="1:130" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:130">
       <c r="CP69" s="2"/>
       <c r="CQ69" s="2"/>
       <c r="CR69" s="2"/>
@@ -42294,7 +42284,7 @@
       <c r="DX69" s="2"/>
       <c r="DZ69" s="9"/>
     </row>
-    <row r="70" spans="1:130" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:130">
       <c r="A70" s="1" t="s">
         <v>67</v>
       </c>
@@ -42717,7 +42707,7 @@
       <c r="DX70" s="2"/>
       <c r="DZ70" s="9"/>
     </row>
-    <row r="71" spans="1:130" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:130">
       <c r="A71" t="s">
         <v>68</v>
       </c>
@@ -42865,7 +42855,7 @@
       <c r="DY71" s="1"/>
       <c r="DZ71" s="9"/>
     </row>
-    <row r="72" spans="1:130" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:130">
       <c r="A72" t="s">
         <v>69</v>
       </c>
@@ -43008,7 +42998,7 @@
       <c r="DX72" s="2"/>
       <c r="DZ72" s="9"/>
     </row>
-    <row r="73" spans="1:130" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:130">
       <c r="CP73" s="2"/>
       <c r="CQ73" s="2"/>
       <c r="CR73" s="2"/>
@@ -43046,7 +43036,7 @@
       <c r="DX73" s="2"/>
       <c r="DZ73" s="9"/>
     </row>
-    <row r="74" spans="1:130" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:130">
       <c r="A74" t="s">
         <v>138</v>
       </c>
@@ -43087,7 +43077,7 @@
       <c r="DX74" s="2"/>
       <c r="DZ74" s="9"/>
     </row>
-    <row r="75" spans="1:130" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:130">
       <c r="A75" t="str">
         <f>A9</f>
         <v>Belgium</v>
@@ -43136,7 +43126,7 @@
       <c r="DX75" s="2"/>
       <c r="DZ75" s="9"/>
     </row>
-    <row r="76" spans="1:130" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:130">
       <c r="A76" t="str">
         <f>A22</f>
         <v>France</v>
@@ -43185,7 +43175,7 @@
       <c r="DX76" s="2"/>
       <c r="DZ76" s="9"/>
     </row>
-    <row r="77" spans="1:130" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:130">
       <c r="A77" s="10" t="str">
         <f>A23</f>
         <v>Germany</v>
@@ -43234,7 +43224,7 @@
       <c r="DX77" s="2"/>
       <c r="DZ77" s="9"/>
     </row>
-    <row r="78" spans="1:130" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:130">
       <c r="A78" t="str">
         <f>A28</f>
         <v>Italy</v>
@@ -43283,7 +43273,7 @@
       <c r="DX78" s="2"/>
       <c r="DZ78" s="9"/>
     </row>
-    <row r="79" spans="1:130" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:130">
       <c r="A79" t="str">
         <f>A42</f>
         <v>Poland</v>
@@ -43332,7 +43322,7 @@
       <c r="DX79" s="2"/>
       <c r="DZ79" s="9"/>
     </row>
-    <row r="80" spans="1:130" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:130">
       <c r="A80" s="45" t="s">
         <v>19</v>
       </c>
@@ -43381,7 +43371,7 @@
       <c r="DW80" s="2"/>
       <c r="DX80" s="2"/>
     </row>
-    <row r="81" spans="1:128" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:128">
       <c r="A81" t="s">
         <v>140</v>
       </c>
@@ -43424,7 +43414,7 @@
       <c r="DW81" s="2"/>
       <c r="DX81" s="2"/>
     </row>
-    <row r="82" spans="1:128" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:128">
       <c r="A82" t="s">
         <v>139</v>
       </c>
@@ -43470,7 +43460,7 @@
       <c r="DW82" s="2"/>
       <c r="DX82" s="2"/>
     </row>
-    <row r="84" spans="1:128" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:128">
       <c r="A84" s="49"/>
       <c r="B84" s="49"/>
       <c r="C84" s="49"/>
@@ -43592,6 +43582,12 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -43607,7 +43603,7 @@
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="19.83203125" style="32" customWidth="1"/>
     <col min="2" max="2" width="7.83203125" style="32" customWidth="1"/>
@@ -43619,12 +43615,12 @@
     <col min="8" max="16384" width="8.83203125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" s="32" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2" s="32" t="s">
         <v>0</v>
       </c>
@@ -43635,7 +43631,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="5" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" s="5" customFormat="1">
       <c r="A3" s="33" t="s">
         <v>1</v>
       </c>
@@ -43655,7 +43651,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8">
       <c r="A4" s="32" t="s">
         <v>2</v>
       </c>
@@ -43679,7 +43675,7 @@
         <v>SPEW</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8">
       <c r="A5" s="32" t="s">
         <v>3</v>
       </c>
@@ -43703,7 +43699,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8">
       <c r="A6" s="32" t="s">
         <v>4</v>
       </c>
@@ -43727,7 +43723,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8">
       <c r="A7" s="32" t="s">
         <v>5</v>
       </c>
@@ -43751,7 +43747,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8">
       <c r="A8" s="32" t="s">
         <v>6</v>
       </c>
@@ -43775,7 +43771,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8">
       <c r="A9" s="32" t="s">
         <v>7</v>
       </c>
@@ -43799,7 +43795,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8">
       <c r="A10" s="32" t="s">
         <v>8</v>
       </c>
@@ -43823,7 +43819,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8">
       <c r="A11" s="32" t="s">
         <v>9</v>
       </c>
@@ -43847,7 +43843,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8">
       <c r="A12" s="32" t="s">
         <v>10</v>
       </c>
@@ -43871,7 +43867,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8">
       <c r="A13" s="32" t="s">
         <v>11</v>
       </c>
@@ -43895,7 +43891,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8">
       <c r="A14" s="32" t="s">
         <v>12</v>
       </c>
@@ -43919,7 +43915,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8">
       <c r="A15" s="32" t="s">
         <v>13</v>
       </c>
@@ -43943,7 +43939,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8">
       <c r="A16" s="32" t="s">
         <v>14</v>
       </c>
@@ -43967,7 +43963,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9">
       <c r="A17" s="32" t="s">
         <v>15</v>
       </c>
@@ -43991,7 +43987,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9">
       <c r="A18" s="32" t="s">
         <v>16</v>
       </c>
@@ -44015,7 +44011,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9">
       <c r="A19" s="32" t="s">
         <v>17</v>
       </c>
@@ -44039,7 +44035,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9">
       <c r="A20" s="32" t="s">
         <v>18</v>
       </c>
@@ -44063,7 +44059,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9">
       <c r="A21" s="32" t="s">
         <v>19</v>
       </c>
@@ -44087,7 +44083,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9">
       <c r="A22" s="32" t="s">
         <v>20</v>
       </c>
@@ -44111,7 +44107,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9">
       <c r="A23" s="32" t="s">
         <v>21</v>
       </c>
@@ -44138,7 +44134,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9">
       <c r="A24" s="32" t="s">
         <v>22</v>
       </c>
@@ -44165,7 +44161,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9">
       <c r="A25" s="32" t="s">
         <v>23</v>
       </c>
@@ -44189,7 +44185,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9">
       <c r="A26" s="32" t="s">
         <v>24</v>
       </c>
@@ -44213,7 +44209,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9">
       <c r="A27" s="32" t="s">
         <v>25</v>
       </c>
@@ -44237,7 +44233,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9">
       <c r="A28" s="32" t="s">
         <v>26</v>
       </c>
@@ -44261,7 +44257,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9">
       <c r="A29" s="32" t="s">
         <v>27</v>
       </c>
@@ -44285,7 +44281,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9">
       <c r="A30" s="32" t="s">
         <v>28</v>
       </c>
@@ -44309,7 +44305,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9">
       <c r="A31" s="32" t="s">
         <v>29</v>
       </c>
@@ -44333,7 +44329,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9">
       <c r="A32" s="32" t="s">
         <v>30</v>
       </c>
@@ -44357,7 +44353,7 @@
         <v>SPEW</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8">
       <c r="A33" s="32" t="s">
         <v>31</v>
       </c>
@@ -44381,7 +44377,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8">
       <c r="A34" s="32" t="s">
         <v>32</v>
       </c>
@@ -44405,7 +44401,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8">
       <c r="A35" s="32" t="s">
         <v>33</v>
       </c>
@@ -44429,7 +44425,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8">
       <c r="A36" s="32" t="s">
         <v>34</v>
       </c>
@@ -44453,7 +44449,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8">
       <c r="A37" s="32" t="s">
         <v>35</v>
       </c>
@@ -44477,7 +44473,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8">
       <c r="A38" s="32" t="s">
         <v>36</v>
       </c>
@@ -44501,7 +44497,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8">
       <c r="A39" s="32" t="s">
         <v>37</v>
       </c>
@@ -44525,7 +44521,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8">
       <c r="A40" s="32" t="s">
         <v>38</v>
       </c>
@@ -44549,7 +44545,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8">
       <c r="A41" s="32" t="s">
         <v>39</v>
       </c>
@@ -44573,7 +44569,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8">
       <c r="A42" s="32" t="s">
         <v>40</v>
       </c>
@@ -44597,7 +44593,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8">
       <c r="A43" s="32" t="s">
         <v>41</v>
       </c>
@@ -44621,7 +44617,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8">
       <c r="A44" s="32" t="s">
         <v>42</v>
       </c>
@@ -44645,7 +44641,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8">
       <c r="A45" s="32" t="s">
         <v>43</v>
       </c>
@@ -44669,7 +44665,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8">
       <c r="A46" s="32" t="s">
         <v>44</v>
       </c>
@@ -44693,7 +44689,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8">
       <c r="A47" s="32" t="s">
         <v>45</v>
       </c>
@@ -44717,7 +44713,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8">
       <c r="A48" s="32" t="s">
         <v>46</v>
       </c>
@@ -44741,7 +44737,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8">
       <c r="A49" s="32" t="s">
         <v>47</v>
       </c>
@@ -44765,7 +44761,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8">
       <c r="A50" s="32" t="s">
         <v>48</v>
       </c>
@@ -44789,7 +44785,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8">
       <c r="A51" s="32" t="s">
         <v>49</v>
       </c>
@@ -44813,7 +44809,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8">
       <c r="A52" s="32" t="s">
         <v>50</v>
       </c>
@@ -44837,7 +44833,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8">
       <c r="A53" s="32" t="s">
         <v>51</v>
       </c>
@@ -44861,7 +44857,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8">
       <c r="A54" s="32" t="s">
         <v>52</v>
       </c>
@@ -44885,7 +44881,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8">
       <c r="A55" s="32" t="s">
         <v>53</v>
       </c>
@@ -44909,7 +44905,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8">
       <c r="A56" s="32" t="s">
         <v>54</v>
       </c>
@@ -44933,7 +44929,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8">
       <c r="A57" s="32" t="s">
         <v>55</v>
       </c>
@@ -44957,7 +44953,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8">
       <c r="A58" s="32" t="s">
         <v>56</v>
       </c>
@@ -44981,7 +44977,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8">
       <c r="A59" s="32" t="s">
         <v>57</v>
       </c>
@@ -45005,7 +45001,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8">
       <c r="A60" s="32" t="s">
         <v>58</v>
       </c>
@@ -45029,7 +45025,7 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8">
       <c r="A61" s="32" t="s">
         <v>59</v>
       </c>
@@ -45053,7 +45049,7 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8">
       <c r="A62" s="32" t="s">
         <v>60</v>
       </c>
@@ -45077,7 +45073,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8">
       <c r="A63" s="37" t="s">
         <v>61</v>
       </c>
@@ -45101,7 +45097,7 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8">
       <c r="A64" s="32" t="s">
         <v>62</v>
       </c>
@@ -45118,7 +45114,7 @@
         <v>478733.7</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6">
       <c r="A65" s="32" t="s">
         <v>71</v>
       </c>
@@ -45135,10 +45131,10 @@
         <v>478787.5</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6">
       <c r="D66" s="36"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6">
       <c r="A67" s="32" t="s">
         <v>66</v>
       </c>
@@ -45151,7 +45147,7 @@
         <v>514000</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6">
       <c r="A68" s="32" t="s">
         <v>70</v>
       </c>
@@ -45164,10 +45160,10 @@
         <v>451657</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6">
       <c r="D69" s="36"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6">
       <c r="A70" s="32" t="s">
         <v>67</v>
       </c>
@@ -45180,7 +45176,7 @@
         <v>62300</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6">
       <c r="A71" s="32" t="s">
         <v>68</v>
       </c>
@@ -45193,7 +45189,7 @@
         <v>62343</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6">
       <c r="A72" s="32" t="s">
         <v>69</v>
       </c>
@@ -45202,16 +45198,16 @@
         <v>1.0006902086677367</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6">
       <c r="D73" s="36"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6">
       <c r="A74" s="32" t="s">
         <v>138</v>
       </c>
       <c r="D74" s="36"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6">
       <c r="A75" s="32" t="str">
         <f>A9</f>
         <v>Belgium</v>
@@ -45225,7 +45221,7 @@
         <v>9844</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6">
       <c r="A76" s="32" t="str">
         <f>A22</f>
         <v>France</v>
@@ -45239,7 +45235,7 @@
         <v>18677</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6">
       <c r="A77" s="32" t="str">
         <f>A23</f>
         <v>Germany</v>
@@ -45253,7 +45249,7 @@
         <v>33609</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6">
       <c r="A78" s="32" t="str">
         <f>A28</f>
         <v>Italy</v>
@@ -45267,7 +45263,7 @@
         <v>12149</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6">
       <c r="A79" s="32" t="str">
         <f>A42</f>
         <v>Poland</v>
@@ -45281,7 +45277,7 @@
         <v>11378</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6">
       <c r="A80" s="32" t="s">
         <v>140</v>
       </c>
@@ -45290,7 +45286,7 @@
         <v>22343</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4">
       <c r="A81" s="32" t="s">
         <v>139</v>
       </c>
@@ -45298,7 +45294,7 @@
         <v>108000</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4">
       <c r="D82" s="36"/>
     </row>
   </sheetData>
@@ -45309,6 +45305,12 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -45321,17 +45323,17 @@
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>65</v>
       </c>
@@ -45339,7 +45341,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>74</v>
       </c>
@@ -45347,12 +45349,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>76</v>
       </c>
@@ -45360,6 +45362,12 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -45377,14 +45385,14 @@
       <selection activeCell="C2" sqref="C2:Q2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="2" width="10.83203125" style="12"/>
     <col min="3" max="17" width="6.33203125" style="12" customWidth="1"/>
     <col min="18" max="16384" width="10.83203125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:37">
       <c r="A1" s="12" t="s">
         <v>141</v>
       </c>
@@ -45491,7 +45499,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:37">
       <c r="A2" s="12" t="s">
         <v>158</v>
       </c>
@@ -45513,7 +45521,7 @@
         <v>Additional</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:37">
       <c r="A3" s="12" t="s">
         <v>159</v>
       </c>
@@ -45595,7 +45603,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:37">
       <c r="A4" s="12" t="s">
         <v>160</v>
       </c>
@@ -45692,7 +45700,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:37">
       <c r="A5" s="12" t="s">
         <v>161</v>
       </c>
@@ -45801,7 +45809,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:37">
       <c r="A6" s="12" t="s">
         <v>162</v>
       </c>
@@ -45910,7 +45918,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:37">
       <c r="A7" s="12" t="s">
         <v>163</v>
       </c>
@@ -46019,7 +46027,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:37">
       <c r="A8" s="12" t="s">
         <v>164</v>
       </c>
@@ -46086,7 +46094,7 @@
         <v>Additional</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:37">
       <c r="A9" s="12" t="s">
         <v>165</v>
       </c>
@@ -46195,7 +46203,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:37">
       <c r="A10" s="12" t="s">
         <v>166</v>
       </c>
@@ -46289,7 +46297,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:37">
       <c r="A11" s="12" t="s">
         <v>167</v>
       </c>
@@ -46398,7 +46406,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:37">
       <c r="A12" s="12" t="s">
         <v>168</v>
       </c>
@@ -46498,7 +46506,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:37">
       <c r="A13" s="12" t="s">
         <v>169</v>
       </c>
@@ -46607,7 +46615,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:37">
       <c r="A14" s="12" t="s">
         <v>170</v>
       </c>
@@ -46698,7 +46706,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:37">
       <c r="A15" s="12" t="s">
         <v>171</v>
       </c>
@@ -46789,7 +46797,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:37">
       <c r="A16" s="12" t="s">
         <v>172</v>
       </c>
@@ -46856,7 +46864,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:37">
       <c r="A17" s="12" t="s">
         <v>173</v>
       </c>
@@ -46959,7 +46967,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:37">
       <c r="A18" s="12" t="s">
         <v>174</v>
       </c>
@@ -47038,7 +47046,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:37">
       <c r="A19" s="12" t="s">
         <v>176</v>
       </c>
@@ -47126,7 +47134,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:37">
       <c r="A20" s="12" t="s">
         <v>177</v>
       </c>
@@ -47235,7 +47243,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:37">
       <c r="A21" s="12" t="s">
         <v>178</v>
       </c>
@@ -47344,7 +47352,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:37">
       <c r="A22" s="12" t="s">
         <v>179</v>
       </c>
@@ -47408,7 +47416,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:37">
       <c r="A23" s="12" t="s">
         <v>181</v>
       </c>
@@ -47484,7 +47492,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:37">
       <c r="A24" s="12" t="s">
         <v>182</v>
       </c>
@@ -47563,7 +47571,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:37">
       <c r="A25" s="12" t="s">
         <v>183</v>
       </c>
@@ -47642,7 +47650,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:37">
       <c r="A26" s="12" t="s">
         <v>184</v>
       </c>
@@ -47751,7 +47759,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:37">
       <c r="A27" s="12" t="s">
         <v>185</v>
       </c>
@@ -47860,7 +47868,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:37">
       <c r="A28" s="12" t="s">
         <v>186</v>
       </c>
@@ -47939,7 +47947,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:37">
       <c r="A29" s="12" t="s">
         <v>187</v>
       </c>
@@ -48048,7 +48056,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:37">
       <c r="A30" s="12" t="s">
         <v>188</v>
       </c>
@@ -48127,7 +48135,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:37">
       <c r="A31" s="12" t="s">
         <v>189</v>
       </c>
@@ -48218,7 +48226,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:37">
       <c r="A32" s="12" t="s">
         <v>190</v>
       </c>
@@ -48285,7 +48293,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:37">
       <c r="A33" s="12" t="s">
         <v>191</v>
       </c>
@@ -48379,7 +48387,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:37">
       <c r="A34" s="12" t="s">
         <v>192</v>
       </c>
@@ -48461,7 +48469,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:37">
       <c r="A35" s="12" t="s">
         <v>193</v>
       </c>
@@ -48567,7 +48575,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:37">
       <c r="A36" s="12" t="s">
         <v>194</v>
       </c>
@@ -48631,7 +48639,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:37">
       <c r="A37" s="12" t="s">
         <v>196</v>
       </c>
@@ -48695,7 +48703,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:37">
       <c r="A38" s="12" t="s">
         <v>197</v>
       </c>
@@ -48804,7 +48812,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:37">
       <c r="A39" s="12" t="s">
         <v>198</v>
       </c>
@@ -48880,7 +48888,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:37">
       <c r="A40" s="12" t="s">
         <v>199</v>
       </c>
@@ -48947,7 +48955,7 @@
         <v>Additional</v>
       </c>
     </row>
-    <row r="41" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:37">
       <c r="A41" s="12" t="s">
         <v>201</v>
       </c>
@@ -49056,7 +49064,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:37">
       <c r="A42" s="12" t="s">
         <v>202</v>
       </c>
@@ -49123,7 +49131,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:37">
       <c r="A43" s="12" t="s">
         <v>203</v>
       </c>
@@ -49199,7 +49207,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:37">
       <c r="A44" s="12" t="s">
         <v>204</v>
       </c>
@@ -49272,7 +49280,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:37">
       <c r="A45" s="12" t="s">
         <v>205</v>
       </c>
@@ -49339,7 +49347,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:37">
       <c r="A46" s="12" t="s">
         <v>206</v>
       </c>
@@ -49427,7 +49435,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:37">
       <c r="A47" s="12" t="s">
         <v>207</v>
       </c>
@@ -49497,7 +49505,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:37">
       <c r="A48" s="12" t="s">
         <v>209</v>
       </c>
@@ -49606,7 +49614,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:37">
       <c r="A49" s="12" t="s">
         <v>210</v>
       </c>
@@ -49682,7 +49690,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:37">
       <c r="A50" s="12" t="s">
         <v>211</v>
       </c>
@@ -49791,7 +49799,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:37">
       <c r="A51" s="12" t="s">
         <v>212</v>
       </c>
@@ -49861,7 +49869,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:37">
       <c r="A52" s="12" t="s">
         <v>213</v>
       </c>
@@ -49928,7 +49936,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:37">
       <c r="A53" s="12" t="s">
         <v>214</v>
       </c>
@@ -49995,7 +50003,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:37">
       <c r="A54" s="12" t="s">
         <v>215</v>
       </c>
@@ -50086,7 +50094,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:37">
       <c r="A55" s="12" t="s">
         <v>216</v>
       </c>
@@ -50195,7 +50203,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:37">
       <c r="A56" s="12" t="s">
         <v>217</v>
       </c>
@@ -50304,7 +50312,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:37">
       <c r="A57" s="12" t="s">
         <v>218</v>
       </c>
@@ -50404,7 +50412,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:37">
       <c r="A58" s="12" t="s">
         <v>219</v>
       </c>
@@ -50468,7 +50476,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:37">
       <c r="A59" s="12" t="s">
         <v>221</v>
       </c>
@@ -50550,7 +50558,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:37">
       <c r="A60" s="12" t="s">
         <v>222</v>
       </c>
@@ -50650,7 +50658,7 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:37">
       <c r="A61" s="12" t="s">
         <v>223</v>
       </c>
@@ -50720,7 +50728,7 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:37">
       <c r="A62" s="12" t="s">
         <v>224</v>
       </c>
@@ -50829,7 +50837,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:37">
       <c r="A63" s="12" t="s">
         <v>225</v>
       </c>
@@ -50905,7 +50913,7 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:37">
       <c r="A64" s="12" t="s">
         <v>226</v>
       </c>
@@ -51014,7 +51022,7 @@
         <v/>
       </c>
     </row>
-    <row r="65" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:37">
       <c r="A65" s="12" t="s">
         <v>227</v>
       </c>
@@ -51114,7 +51122,7 @@
         <v/>
       </c>
     </row>
-    <row r="66" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:37">
       <c r="A66" s="12" t="s">
         <v>228</v>
       </c>
@@ -51193,7 +51201,7 @@
         <v/>
       </c>
     </row>
-    <row r="67" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:37">
       <c r="A67" s="12" t="s">
         <v>229</v>
       </c>
@@ -51260,7 +51268,7 @@
         <v/>
       </c>
     </row>
-    <row r="68" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:37">
       <c r="A68" s="12" t="s">
         <v>230</v>
       </c>
@@ -51363,7 +51371,7 @@
         <v/>
       </c>
     </row>
-    <row r="69" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:37">
       <c r="A69" s="12" t="s">
         <v>231</v>
       </c>
@@ -51406,6 +51414,12 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -51425,7 +51439,7 @@
       <selection pane="bottomLeft" activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.6640625" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="20.83203125" style="14" customWidth="1"/>
     <col min="2" max="2" width="10" style="14" customWidth="1"/>
@@ -51434,7 +51448,7 @@
     <col min="25" max="16384" width="14.6640625" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:43">
       <c r="A1" s="13" t="s">
         <v>232</v>
       </c>
@@ -51443,7 +51457,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:43">
       <c r="AA2" s="14">
         <v>1890</v>
       </c>
@@ -51496,7 +51510,7 @@
         <v>1969</v>
       </c>
     </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:43">
       <c r="A3" s="16"/>
       <c r="B3" s="16"/>
       <c r="C3" s="17">
@@ -51625,7 +51639,7 @@
         <v>109545</v>
       </c>
     </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:43">
       <c r="C4" s="18"/>
       <c r="D4" s="18"/>
       <c r="E4" s="18"/>
@@ -51702,7 +51716,7 @@
         <v>21523</v>
       </c>
     </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:43">
       <c r="A5" s="15" t="s">
         <v>11</v>
       </c>
@@ -51834,7 +51848,7 @@
         <v>81634</v>
       </c>
     </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:43">
       <c r="A6" s="15" t="s">
         <v>237</v>
       </c>
@@ -51905,7 +51919,7 @@
       <c r="X6" s="20"/>
       <c r="Y6" s="20"/>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:43">
       <c r="A7" s="15" t="s">
         <v>238</v>
       </c>
@@ -51998,7 +52012,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:43">
       <c r="A8" s="15" t="s">
         <v>240</v>
       </c>
@@ -52089,7 +52103,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:43">
       <c r="A9" s="15" t="s">
         <v>242</v>
       </c>
@@ -52184,7 +52198,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="10" spans="1:43" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:43">
       <c r="A10" s="15" t="s">
         <v>244</v>
       </c>
@@ -52269,7 +52283,7 @@
       <c r="X10" s="22"/>
       <c r="Y10" s="20"/>
     </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:43">
       <c r="A11" s="15" t="s">
         <v>246</v>
       </c>
@@ -52340,7 +52354,7 @@
       <c r="X11" s="20"/>
       <c r="Y11" s="20"/>
     </row>
-    <row r="12" spans="1:43" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:43">
       <c r="A12" s="15" t="s">
         <v>247</v>
       </c>
@@ -52416,7 +52430,7 @@
       <c r="X12" s="22"/>
       <c r="Y12" s="20"/>
     </row>
-    <row r="13" spans="1:43" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:43">
       <c r="A13" s="15" t="s">
         <v>248</v>
       </c>
@@ -52487,7 +52501,7 @@
       <c r="X13" s="20"/>
       <c r="Y13" s="20"/>
     </row>
-    <row r="14" spans="1:43" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:43">
       <c r="A14" s="15" t="s">
         <v>249</v>
       </c>
@@ -52568,7 +52582,7 @@
       <c r="X14" s="20"/>
       <c r="Y14" s="20"/>
     </row>
-    <row r="15" spans="1:43" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:43">
       <c r="A15" s="15" t="s">
         <v>250</v>
       </c>
@@ -52649,7 +52663,7 @@
       <c r="X15" s="22"/>
       <c r="Y15" s="20"/>
     </row>
-    <row r="16" spans="1:43" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:43">
       <c r="A16" s="15" t="s">
         <v>251</v>
       </c>
@@ -52723,7 +52737,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:25">
       <c r="A17" s="15" t="s">
         <v>27</v>
       </c>
@@ -52794,7 +52808,7 @@
       <c r="X17" s="22"/>
       <c r="Y17" s="20"/>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:25">
       <c r="C18" s="19"/>
       <c r="D18" s="19"/>
       <c r="E18" s="19"/>
@@ -52819,7 +52833,7 @@
       <c r="X18" s="20"/>
       <c r="Y18" s="20"/>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:25">
       <c r="A19" s="24" t="s">
         <v>253</v>
       </c>
@@ -52911,7 +52925,7 @@
       <c r="X19" s="20"/>
       <c r="Y19" s="20"/>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:25">
       <c r="C20" s="19"/>
       <c r="D20" s="19"/>
       <c r="E20" s="19"/>
@@ -52936,7 +52950,7 @@
       <c r="X20" s="20"/>
       <c r="Y20" s="20"/>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:25">
       <c r="A21" s="25" t="s">
         <v>254</v>
       </c>
@@ -52965,7 +52979,7 @@
       <c r="X21" s="20"/>
       <c r="Y21" s="20"/>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:25">
       <c r="A22" s="15" t="s">
         <v>255</v>
       </c>
@@ -53036,7 +53050,7 @@
       <c r="X22" s="22"/>
       <c r="Y22" s="20"/>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:25">
       <c r="A23" s="16" t="s">
         <v>256</v>
       </c>
@@ -53106,7 +53120,7 @@
       </c>
       <c r="X23" s="27"/>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:25">
       <c r="C24" s="18"/>
       <c r="D24" s="18"/>
       <c r="E24" s="18"/>
@@ -53130,7 +53144,7 @@
       <c r="W24" s="18"/>
       <c r="X24" s="28"/>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:25">
       <c r="A25" s="29" t="s">
         <v>257</v>
       </c>
@@ -53157,7 +53171,7 @@
       <c r="V25" s="18"/>
       <c r="W25" s="18"/>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:25">
       <c r="C26" s="18"/>
       <c r="D26" s="18"/>
       <c r="E26" s="18"/>
@@ -53180,7 +53194,7 @@
       <c r="V26" s="18"/>
       <c r="W26" s="18"/>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:25">
       <c r="A27" s="15" t="s">
         <v>258</v>
       </c>
@@ -53207,7 +53221,7 @@
       <c r="V27" s="18"/>
       <c r="W27" s="18"/>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:25">
       <c r="A28" s="29" t="s">
         <v>259</v>
       </c>
@@ -53234,7 +53248,7 @@
       <c r="V28" s="18"/>
       <c r="W28" s="18"/>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:25">
       <c r="A29" s="30" t="s">
         <v>260</v>
       </c>
@@ -53261,7 +53275,7 @@
       <c r="V29" s="18"/>
       <c r="W29" s="18"/>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:25">
       <c r="C30" s="18"/>
       <c r="D30" s="18"/>
       <c r="E30" s="18"/>
@@ -53284,7 +53298,7 @@
       <c r="V30" s="18"/>
       <c r="W30" s="18"/>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:25">
       <c r="C31" s="18"/>
       <c r="D31" s="18"/>
       <c r="E31" s="18"/>
@@ -53307,7 +53321,7 @@
       <c r="V31" s="18"/>
       <c r="W31" s="18"/>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:25">
       <c r="A32" s="13" t="s">
         <v>261</v>
       </c>
@@ -53334,7 +53348,7 @@
       <c r="V32" s="18"/>
       <c r="W32" s="18"/>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:25">
       <c r="C33" s="18"/>
       <c r="D33" s="18"/>
       <c r="E33" s="18"/>
@@ -53357,7 +53371,7 @@
       <c r="V33" s="18"/>
       <c r="W33" s="18"/>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:25">
       <c r="B34" s="14" t="s">
         <v>268</v>
       </c>
@@ -53432,7 +53446,7 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:25">
       <c r="C35" s="18"/>
       <c r="D35" s="18"/>
       <c r="E35" s="18"/>
@@ -53455,7 +53469,7 @@
       <c r="V35" s="18"/>
       <c r="W35" s="18"/>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:25">
       <c r="A36" s="15" t="s">
         <v>11</v>
       </c>
@@ -53526,7 +53540,7 @@
       <c r="X36" s="22"/>
       <c r="Y36" s="20"/>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:25">
       <c r="A37" s="15" t="s">
         <v>237</v>
       </c>
@@ -53597,7 +53611,7 @@
       <c r="X37" s="20"/>
       <c r="Y37" s="20"/>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:25">
       <c r="A38" s="15" t="s">
         <v>238</v>
       </c>
@@ -53684,7 +53698,7 @@
       <c r="X38" s="22"/>
       <c r="Y38" s="20"/>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:25">
       <c r="A39" s="15" t="s">
         <v>240</v>
       </c>
@@ -53764,7 +53778,7 @@
       <c r="X39" s="22"/>
       <c r="Y39" s="20"/>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:25">
       <c r="A40" s="15" t="s">
         <v>242</v>
       </c>
@@ -53849,7 +53863,7 @@
       <c r="X40" s="22"/>
       <c r="Y40" s="20"/>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:25">
       <c r="A41" s="15" t="s">
         <v>244</v>
       </c>
@@ -53933,7 +53947,7 @@
       <c r="X41" s="22"/>
       <c r="Y41" s="20"/>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:25">
       <c r="A42" s="15" t="s">
         <v>246</v>
       </c>
@@ -54004,7 +54018,7 @@
       <c r="X42" s="22"/>
       <c r="Y42" s="20"/>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:25">
       <c r="A43" s="15" t="s">
         <v>247</v>
       </c>
@@ -54078,7 +54092,7 @@
       <c r="X43" s="22"/>
       <c r="Y43" s="20"/>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:25">
       <c r="A44" s="15" t="s">
         <v>248</v>
       </c>
@@ -54151,7 +54165,7 @@
       <c r="X44" s="22"/>
       <c r="Y44" s="20"/>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:25">
       <c r="A45" s="15" t="s">
         <v>249</v>
       </c>
@@ -54234,7 +54248,7 @@
       <c r="X45" s="20"/>
       <c r="Y45" s="20"/>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:25">
       <c r="A46" s="15" t="s">
         <v>250</v>
       </c>
@@ -54308,7 +54322,7 @@
       <c r="X46" s="22"/>
       <c r="Y46" s="20"/>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:25">
       <c r="A47" s="15" t="s">
         <v>251</v>
       </c>
@@ -54379,7 +54393,7 @@
       <c r="X47" s="22"/>
       <c r="Y47" s="20"/>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:25">
       <c r="A48" s="15" t="s">
         <v>27</v>
       </c>
@@ -54450,7 +54464,7 @@
       <c r="X48" s="20"/>
       <c r="Y48" s="20"/>
     </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:25">
       <c r="C49" s="19"/>
       <c r="D49" s="19"/>
       <c r="E49" s="19"/>
@@ -54475,7 +54489,7 @@
       <c r="X49" s="20"/>
       <c r="Y49" s="20"/>
     </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:25">
       <c r="A50" s="24" t="s">
         <v>253</v>
       </c>
@@ -54567,7 +54581,7 @@
       <c r="X50" s="20"/>
       <c r="Y50" s="20"/>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:25">
       <c r="C51" s="19"/>
       <c r="D51" s="19"/>
       <c r="E51" s="19"/>
@@ -54592,7 +54606,7 @@
       <c r="X51" s="20"/>
       <c r="Y51" s="20"/>
     </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:25">
       <c r="A52" s="25" t="s">
         <v>254</v>
       </c>
@@ -54621,7 +54635,7 @@
       <c r="X52" s="20"/>
       <c r="Y52" s="20"/>
     </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:25">
       <c r="A53" s="15" t="s">
         <v>262</v>
       </c>
@@ -54692,7 +54706,7 @@
       <c r="X53" s="20"/>
       <c r="Y53" s="20"/>
     </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:25">
       <c r="A54" s="15" t="s">
         <v>263</v>
       </c>
@@ -54723,7 +54737,7 @@
       <c r="X54" s="20"/>
       <c r="Y54" s="20"/>
     </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:25">
       <c r="C55" s="18"/>
       <c r="D55" s="18"/>
       <c r="E55" s="18"/>
@@ -54746,7 +54760,7 @@
       <c r="V55" s="18"/>
       <c r="W55" s="18"/>
     </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:25">
       <c r="A56" s="29" t="s">
         <v>264</v>
       </c>
@@ -54773,7 +54787,7 @@
       <c r="V56" s="18"/>
       <c r="W56" s="18"/>
     </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:25">
       <c r="A57" s="15"/>
       <c r="B57" s="15"/>
       <c r="C57" s="18"/>
@@ -54798,7 +54812,7 @@
       <c r="V57" s="18"/>
       <c r="W57" s="18"/>
     </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:25">
       <c r="A58" s="29" t="s">
         <v>259</v>
       </c>
@@ -54825,7 +54839,7 @@
       <c r="V58" s="18"/>
       <c r="W58" s="18"/>
     </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:25">
       <c r="A59" s="15" t="s">
         <v>265</v>
       </c>
@@ -54852,7 +54866,7 @@
       <c r="V59" s="18"/>
       <c r="W59" s="18"/>
     </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:25">
       <c r="A60" s="30" t="s">
         <v>266</v>
       </c>
@@ -54879,7 +54893,7 @@
       <c r="V60" s="18"/>
       <c r="W60" s="18"/>
     </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:25">
       <c r="C61" s="18"/>
       <c r="D61" s="18"/>
       <c r="E61" s="18"/>
@@ -54902,7 +54916,7 @@
       <c r="V61" s="18"/>
       <c r="W61" s="18"/>
     </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:25">
       <c r="A62" s="13" t="s">
         <v>267</v>
       </c>
@@ -54929,7 +54943,7 @@
       <c r="V62" s="18"/>
       <c r="W62" s="18"/>
     </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:25">
       <c r="C63" s="18"/>
       <c r="D63" s="18"/>
       <c r="E63" s="18"/>
@@ -54952,7 +54966,7 @@
       <c r="V63" s="18"/>
       <c r="W63" s="18"/>
     </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:25">
       <c r="A64" s="15" t="s">
         <v>268</v>
       </c>
@@ -55028,7 +55042,7 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="65" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:24">
       <c r="C65" s="18"/>
       <c r="D65" s="18"/>
       <c r="E65" s="18"/>
@@ -55051,7 +55065,7 @@
       <c r="V65" s="18"/>
       <c r="W65" s="18"/>
     </row>
-    <row r="66" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:24">
       <c r="A66" s="15" t="s">
         <v>11</v>
       </c>
@@ -55121,7 +55135,7 @@
       </c>
       <c r="X66" s="22"/>
     </row>
-    <row r="67" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:24">
       <c r="A67" s="15" t="s">
         <v>237</v>
       </c>
@@ -55191,7 +55205,7 @@
       </c>
       <c r="X67" s="22"/>
     </row>
-    <row r="68" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:24">
       <c r="A68" s="15" t="s">
         <v>238</v>
       </c>
@@ -55261,7 +55275,7 @@
       </c>
       <c r="X68" s="22"/>
     </row>
-    <row r="69" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:24">
       <c r="A69" s="15" t="s">
         <v>240</v>
       </c>
@@ -55331,7 +55345,7 @@
       </c>
       <c r="X69" s="22"/>
     </row>
-    <row r="70" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:24">
       <c r="A70" s="15" t="s">
         <v>242</v>
       </c>
@@ -55401,7 +55415,7 @@
       </c>
       <c r="X70" s="22"/>
     </row>
-    <row r="71" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:24">
       <c r="A71" s="15" t="s">
         <v>244</v>
       </c>
@@ -55471,7 +55485,7 @@
       </c>
       <c r="X71" s="22"/>
     </row>
-    <row r="72" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:24">
       <c r="A72" s="15" t="s">
         <v>246</v>
       </c>
@@ -55541,7 +55555,7 @@
       </c>
       <c r="X72" s="22"/>
     </row>
-    <row r="73" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:24">
       <c r="A73" s="15" t="s">
         <v>247</v>
       </c>
@@ -55611,7 +55625,7 @@
       </c>
       <c r="X73" s="22"/>
     </row>
-    <row r="74" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:24">
       <c r="A74" s="15" t="s">
         <v>248</v>
       </c>
@@ -55681,7 +55695,7 @@
       </c>
       <c r="X74" s="22"/>
     </row>
-    <row r="75" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:24">
       <c r="A75" s="15" t="s">
         <v>249</v>
       </c>
@@ -55751,7 +55765,7 @@
       </c>
       <c r="X75" s="22"/>
     </row>
-    <row r="76" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:24">
       <c r="A76" s="15" t="s">
         <v>250</v>
       </c>
@@ -55821,7 +55835,7 @@
       </c>
       <c r="X76" s="22"/>
     </row>
-    <row r="77" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:24">
       <c r="A77" s="15" t="s">
         <v>251</v>
       </c>
@@ -55891,7 +55905,7 @@
       </c>
       <c r="X77" s="22"/>
     </row>
-    <row r="78" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:24">
       <c r="A78" s="15" t="s">
         <v>27</v>
       </c>
@@ -55961,7 +55975,7 @@
       </c>
       <c r="X78" s="22"/>
     </row>
-    <row r="79" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:24">
       <c r="C79" s="18"/>
       <c r="D79" s="18"/>
       <c r="E79" s="18"/>
@@ -55984,7 +55998,7 @@
       <c r="V79" s="18"/>
       <c r="W79" s="18"/>
     </row>
-    <row r="80" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:24">
       <c r="A80" s="24" t="s">
         <v>253</v>
       </c>
@@ -56075,7 +56089,7 @@
       </c>
       <c r="X80" s="20"/>
     </row>
-    <row r="81" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:24">
       <c r="C81" s="18"/>
       <c r="D81" s="18"/>
       <c r="E81" s="18"/>
@@ -56098,7 +56112,7 @@
       <c r="V81" s="18"/>
       <c r="W81" s="18"/>
     </row>
-    <row r="82" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:24">
       <c r="C82" s="18"/>
       <c r="D82" s="18"/>
       <c r="E82" s="18"/>
@@ -56121,7 +56135,7 @@
       <c r="V82" s="18"/>
       <c r="W82" s="18"/>
     </row>
-    <row r="83" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:24">
       <c r="C83" s="18"/>
       <c r="D83" s="18"/>
       <c r="E83" s="18"/>
@@ -56144,7 +56158,7 @@
       <c r="V83" s="18"/>
       <c r="W83" s="18"/>
     </row>
-    <row r="84" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:24">
       <c r="A84" s="13" t="s">
         <v>269</v>
       </c>
@@ -56171,7 +56185,7 @@
       <c r="V84" s="18"/>
       <c r="W84" s="18"/>
     </row>
-    <row r="85" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:24">
       <c r="C85" s="18"/>
       <c r="D85" s="18"/>
       <c r="E85" s="18"/>
@@ -56194,7 +56208,7 @@
       <c r="V85" s="18"/>
       <c r="W85" s="18"/>
     </row>
-    <row r="86" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:24">
       <c r="A86" s="15" t="s">
         <v>268</v>
       </c>
@@ -56270,7 +56284,7 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="87" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:24">
       <c r="C87" s="18"/>
       <c r="D87" s="18"/>
       <c r="E87" s="18"/>
@@ -56293,7 +56307,7 @@
       <c r="V87" s="18"/>
       <c r="W87" s="18"/>
     </row>
-    <row r="88" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:24">
       <c r="A88" s="15" t="s">
         <v>11</v>
       </c>
@@ -56363,7 +56377,7 @@
       </c>
       <c r="X88" s="22"/>
     </row>
-    <row r="89" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:24">
       <c r="A89" s="15" t="s">
         <v>237</v>
       </c>
@@ -56433,7 +56447,7 @@
       </c>
       <c r="X89" s="20"/>
     </row>
-    <row r="90" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:24">
       <c r="A90" s="15" t="s">
         <v>238</v>
       </c>
@@ -56503,7 +56517,7 @@
       </c>
       <c r="X90" s="22"/>
     </row>
-    <row r="91" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:24">
       <c r="A91" s="15" t="s">
         <v>240</v>
       </c>
@@ -56573,7 +56587,7 @@
       </c>
       <c r="X91" s="22"/>
     </row>
-    <row r="92" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:24">
       <c r="A92" s="15" t="s">
         <v>242</v>
       </c>
@@ -56643,7 +56657,7 @@
       </c>
       <c r="X92" s="22"/>
     </row>
-    <row r="93" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:24">
       <c r="A93" s="15" t="s">
         <v>244</v>
       </c>
@@ -56713,7 +56727,7 @@
       </c>
       <c r="X93" s="22"/>
     </row>
-    <row r="94" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:24">
       <c r="A94" s="15" t="s">
         <v>246</v>
       </c>
@@ -56783,7 +56797,7 @@
       </c>
       <c r="X94" s="20"/>
     </row>
-    <row r="95" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:24">
       <c r="A95" s="15" t="s">
         <v>247</v>
       </c>
@@ -56853,7 +56867,7 @@
       </c>
       <c r="X95" s="22"/>
     </row>
-    <row r="96" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:24">
       <c r="A96" s="15" t="s">
         <v>248</v>
       </c>
@@ -56923,7 +56937,7 @@
       </c>
       <c r="X96" s="22"/>
     </row>
-    <row r="97" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:24">
       <c r="A97" s="15" t="s">
         <v>249</v>
       </c>
@@ -56993,7 +57007,7 @@
       </c>
       <c r="X97" s="20"/>
     </row>
-    <row r="98" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:24">
       <c r="A98" s="15" t="s">
         <v>250</v>
       </c>
@@ -57063,7 +57077,7 @@
       </c>
       <c r="X98" s="22"/>
     </row>
-    <row r="99" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:24">
       <c r="A99" s="15" t="s">
         <v>251</v>
       </c>
@@ -57133,7 +57147,7 @@
       </c>
       <c r="X99" s="22"/>
     </row>
-    <row r="100" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:24">
       <c r="A100" s="15" t="s">
         <v>27</v>
       </c>
@@ -57203,7 +57217,7 @@
       </c>
       <c r="X100" s="20"/>
     </row>
-    <row r="101" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:24">
       <c r="C101" s="18"/>
       <c r="D101" s="18"/>
       <c r="E101" s="18"/>
@@ -57226,7 +57240,7 @@
       <c r="V101" s="18"/>
       <c r="W101" s="18"/>
     </row>
-    <row r="102" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:24">
       <c r="A102" s="24" t="s">
         <v>253</v>
       </c>
@@ -57317,7 +57331,7 @@
       </c>
       <c r="X102" s="20"/>
     </row>
-    <row r="103" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:24">
       <c r="C103" s="18"/>
       <c r="D103" s="18"/>
       <c r="E103" s="18"/>
@@ -57340,7 +57354,7 @@
       <c r="V103" s="18"/>
       <c r="W103" s="18"/>
     </row>
-    <row r="104" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:24">
       <c r="A104" s="25" t="s">
         <v>254</v>
       </c>
@@ -57367,7 +57381,7 @@
       <c r="V104" s="18"/>
       <c r="W104" s="18"/>
     </row>
-    <row r="105" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:24">
       <c r="A105" s="15" t="s">
         <v>270</v>
       </c>
@@ -57437,7 +57451,7 @@
       </c>
       <c r="X105" s="20"/>
     </row>
-    <row r="106" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:24">
       <c r="C106" s="18"/>
       <c r="D106" s="18"/>
       <c r="E106" s="18"/>
@@ -57460,7 +57474,7 @@
       <c r="V106" s="18"/>
       <c r="W106" s="18"/>
     </row>
-    <row r="107" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:24">
       <c r="A107" s="15" t="s">
         <v>271</v>
       </c>
@@ -57487,7 +57501,7 @@
       <c r="V107" s="18"/>
       <c r="W107" s="18"/>
     </row>
-    <row r="108" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:24">
       <c r="A108" s="14" t="s">
         <v>272</v>
       </c>
@@ -57513,7 +57527,7 @@
       <c r="V108" s="18"/>
       <c r="W108" s="18"/>
     </row>
-    <row r="109" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:24">
       <c r="C109" s="18"/>
       <c r="D109" s="18"/>
       <c r="E109" s="18"/>
@@ -57536,7 +57550,7 @@
       <c r="V109" s="18"/>
       <c r="W109" s="18"/>
     </row>
-    <row r="110" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:24">
       <c r="C110" s="18"/>
       <c r="D110" s="18"/>
       <c r="E110" s="18"/>
@@ -57559,7 +57573,7 @@
       <c r="V110" s="18"/>
       <c r="W110" s="18"/>
     </row>
-    <row r="111" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="111" spans="1:24">
       <c r="C111" s="18"/>
       <c r="D111" s="18"/>
       <c r="E111" s="18"/>
@@ -57582,7 +57596,7 @@
       <c r="V111" s="18"/>
       <c r="W111" s="18"/>
     </row>
-    <row r="112" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="112" spans="1:24">
       <c r="A112" s="15" t="s">
         <v>273</v>
       </c>
@@ -57609,7 +57623,7 @@
       <c r="V112" s="18"/>
       <c r="W112" s="18"/>
     </row>
-    <row r="113" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="113" spans="1:23">
       <c r="C113" s="18"/>
       <c r="D113" s="18"/>
       <c r="E113" s="18"/>
@@ -57632,7 +57646,7 @@
       <c r="V113" s="18"/>
       <c r="W113" s="18"/>
     </row>
-    <row r="114" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="114" spans="1:23">
       <c r="A114" s="15" t="s">
         <v>268</v>
       </c>
@@ -57663,7 +57677,7 @@
       <c r="V114" s="18"/>
       <c r="W114" s="18"/>
     </row>
-    <row r="115" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="115" spans="1:23">
       <c r="C115" s="18"/>
       <c r="D115" s="18"/>
       <c r="E115" s="18"/>
@@ -57686,7 +57700,7 @@
       <c r="V115" s="18"/>
       <c r="W115" s="18"/>
     </row>
-    <row r="116" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="116" spans="1:23">
       <c r="A116" s="15" t="s">
         <v>11</v>
       </c>
@@ -57717,7 +57731,7 @@
       <c r="V116" s="18"/>
       <c r="W116" s="18"/>
     </row>
-    <row r="117" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="117" spans="1:23">
       <c r="A117" s="15" t="s">
         <v>237</v>
       </c>
@@ -57748,7 +57762,7 @@
       <c r="V117" s="18"/>
       <c r="W117" s="18"/>
     </row>
-    <row r="118" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="118" spans="1:23">
       <c r="A118" s="15" t="s">
         <v>238</v>
       </c>
@@ -57779,7 +57793,7 @@
       <c r="V118" s="18"/>
       <c r="W118" s="18"/>
     </row>
-    <row r="119" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="119" spans="1:23">
       <c r="A119" s="15" t="s">
         <v>240</v>
       </c>
@@ -57810,7 +57824,7 @@
       <c r="V119" s="18"/>
       <c r="W119" s="18"/>
     </row>
-    <row r="120" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="120" spans="1:23">
       <c r="A120" s="15" t="s">
         <v>242</v>
       </c>
@@ -57841,7 +57855,7 @@
       <c r="V120" s="18"/>
       <c r="W120" s="18"/>
     </row>
-    <row r="121" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="121" spans="1:23">
       <c r="A121" s="15" t="s">
         <v>244</v>
       </c>
@@ -57872,7 +57886,7 @@
       <c r="V121" s="18"/>
       <c r="W121" s="18"/>
     </row>
-    <row r="122" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="122" spans="1:23">
       <c r="A122" s="15" t="s">
         <v>246</v>
       </c>
@@ -57903,7 +57917,7 @@
       <c r="V122" s="18"/>
       <c r="W122" s="18"/>
     </row>
-    <row r="123" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="123" spans="1:23">
       <c r="A123" s="15" t="s">
         <v>247</v>
       </c>
@@ -57934,7 +57948,7 @@
       <c r="V123" s="18"/>
       <c r="W123" s="18"/>
     </row>
-    <row r="124" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="124" spans="1:23">
       <c r="A124" s="15" t="s">
         <v>248</v>
       </c>
@@ -57965,7 +57979,7 @@
       <c r="V124" s="18"/>
       <c r="W124" s="18"/>
     </row>
-    <row r="125" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="125" spans="1:23">
       <c r="A125" s="15" t="s">
         <v>249</v>
       </c>
@@ -57996,7 +58010,7 @@
       <c r="V125" s="18"/>
       <c r="W125" s="18"/>
     </row>
-    <row r="126" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="126" spans="1:23">
       <c r="A126" s="15" t="s">
         <v>250</v>
       </c>
@@ -58027,7 +58041,7 @@
       <c r="V126" s="18"/>
       <c r="W126" s="18"/>
     </row>
-    <row r="127" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="127" spans="1:23">
       <c r="A127" s="15" t="s">
         <v>251</v>
       </c>
@@ -58058,7 +58072,7 @@
       <c r="V127" s="18"/>
       <c r="W127" s="18"/>
     </row>
-    <row r="128" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="128" spans="1:23">
       <c r="A128" s="15" t="s">
         <v>27</v>
       </c>
@@ -58089,7 +58103,7 @@
       <c r="V128" s="18"/>
       <c r="W128" s="18"/>
     </row>
-    <row r="129" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="129" spans="1:24">
       <c r="C129" s="19"/>
       <c r="D129" s="19"/>
       <c r="E129" s="18"/>
@@ -58112,7 +58126,7 @@
       <c r="V129" s="18"/>
       <c r="W129" s="18"/>
     </row>
-    <row r="130" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="130" spans="1:24">
       <c r="A130" s="24" t="s">
         <v>253</v>
       </c>
@@ -58145,7 +58159,7 @@
       <c r="V130" s="18"/>
       <c r="W130" s="18"/>
     </row>
-    <row r="131" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="131" spans="1:24">
       <c r="C131" s="19"/>
       <c r="D131" s="19"/>
       <c r="E131" s="18"/>
@@ -58168,7 +58182,7 @@
       <c r="V131" s="18"/>
       <c r="W131" s="18"/>
     </row>
-    <row r="132" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="132" spans="1:24">
       <c r="A132" s="15" t="s">
         <v>274</v>
       </c>
@@ -58199,7 +58213,7 @@
       <c r="V132" s="18"/>
       <c r="W132" s="18"/>
     </row>
-    <row r="133" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="133" spans="1:24">
       <c r="C133" s="18"/>
       <c r="D133" s="18"/>
       <c r="E133" s="18"/>
@@ -58222,7 +58236,7 @@
       <c r="V133" s="18"/>
       <c r="W133" s="18"/>
     </row>
-    <row r="134" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="134" spans="1:24">
       <c r="A134" s="15" t="s">
         <v>275</v>
       </c>
@@ -58249,7 +58263,7 @@
       <c r="V134" s="18"/>
       <c r="W134" s="18"/>
     </row>
-    <row r="135" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="135" spans="1:24">
       <c r="C135" s="18"/>
       <c r="D135" s="18"/>
       <c r="E135" s="18"/>
@@ -58272,7 +58286,7 @@
       <c r="V135" s="18"/>
       <c r="W135" s="18"/>
     </row>
-    <row r="136" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="136" spans="1:24">
       <c r="A136" s="15" t="s">
         <v>276</v>
       </c>
@@ -58299,7 +58313,7 @@
       <c r="V136" s="18"/>
       <c r="W136" s="18"/>
     </row>
-    <row r="137" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="137" spans="1:24">
       <c r="C137" s="18"/>
       <c r="D137" s="18"/>
       <c r="E137" s="18"/>
@@ -58322,7 +58336,7 @@
       <c r="V137" s="18"/>
       <c r="W137" s="18"/>
     </row>
-    <row r="138" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="138" spans="1:24">
       <c r="C138" s="18"/>
       <c r="D138" s="18"/>
       <c r="E138" s="18"/>
@@ -58345,7 +58359,7 @@
       <c r="V138" s="18"/>
       <c r="W138" s="18"/>
     </row>
-    <row r="139" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="139" spans="1:24">
       <c r="C139" s="18"/>
       <c r="D139" s="18"/>
       <c r="E139" s="18"/>
@@ -58368,7 +58382,7 @@
       <c r="V139" s="18"/>
       <c r="W139" s="18"/>
     </row>
-    <row r="140" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="140" spans="1:24">
       <c r="C140" s="18"/>
       <c r="D140" s="18"/>
       <c r="E140" s="18"/>
@@ -58391,7 +58405,7 @@
       <c r="V140" s="18"/>
       <c r="W140" s="18"/>
     </row>
-    <row r="141" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="141" spans="1:24">
       <c r="A141" s="13" t="s">
         <v>277</v>
       </c>
@@ -58418,7 +58432,7 @@
       <c r="V141" s="18"/>
       <c r="W141" s="18"/>
     </row>
-    <row r="142" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="142" spans="1:24">
       <c r="C142" s="18"/>
       <c r="D142" s="18"/>
       <c r="E142" s="18"/>
@@ -58441,7 +58455,7 @@
       <c r="V142" s="18"/>
       <c r="W142" s="18"/>
     </row>
-    <row r="143" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="143" spans="1:24">
       <c r="C143" s="18">
         <v>1890</v>
       </c>
@@ -58506,7 +58520,7 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="144" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="144" spans="1:24">
       <c r="A144" s="22" t="s">
         <v>278</v>
       </c>
@@ -58597,7 +58611,7 @@
       </c>
       <c r="X144" s="20"/>
     </row>
-    <row r="145" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="145" spans="1:24">
       <c r="A145" s="24" t="s">
         <v>279</v>
       </c>
@@ -58688,7 +58702,7 @@
       </c>
       <c r="X145" s="31"/>
     </row>
-    <row r="146" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="146" spans="1:24">
       <c r="A146" s="24" t="s">
         <v>280</v>
       </c>
@@ -58716,7 +58730,7 @@
       <c r="W146" s="18"/>
       <c r="X146" s="31"/>
     </row>
-    <row r="147" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="147" spans="1:24">
       <c r="A147" s="24" t="s">
         <v>281</v>
       </c>
@@ -58764,5 +58778,11 @@
     <oddFooter>Page &amp;P</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>